<commit_message>
Add initial implementation of database operations and example JSON files
</commit_message>
<xml_diff>
--- a/docs/fhir2sql_data_dictionary.xlsx
+++ b/docs/fhir2sql_data_dictionary.xlsx
@@ -5,26 +5,27 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bertrico/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bertrico/Desktop/fhir2sql/fhir2sql/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066486B8-E7F1-E940-A481-489A6CEE6C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5295EDB9-16FC-EE46-A110-9A75E8A5D2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="660" windowWidth="34140" windowHeight="26280" activeTab="2" xr2:uid="{BC0EC3EA-07AD-0D4D-88B4-AE2E483805A4}"/>
+    <workbookView xWindow="140" yWindow="500" windowWidth="34140" windowHeight="19400" xr2:uid="{BC0EC3EA-07AD-0D4D-88B4-AE2E483805A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="12" r:id="rId1"/>
-    <sheet name="condition" sheetId="3" r:id="rId2"/>
-    <sheet name="documentation_reference" sheetId="7" r:id="rId3"/>
-    <sheet name="encounter" sheetId="1" r:id="rId4"/>
-    <sheet name="immunization" sheetId="10" r:id="rId5"/>
-    <sheet name="medication_statement" sheetId="5" r:id="rId6"/>
-    <sheet name="observation" sheetId="4" r:id="rId7"/>
-    <sheet name="organization" sheetId="9" r:id="rId8"/>
-    <sheet name="patient" sheetId="2" r:id="rId9"/>
-    <sheet name="practitioner" sheetId="8" r:id="rId10"/>
-    <sheet name="procedure" sheetId="6" r:id="rId11"/>
-    <sheet name="provenance" sheetId="11" r:id="rId12"/>
+    <sheet name="claim" sheetId="13" r:id="rId2"/>
+    <sheet name="condition_resource" sheetId="3" r:id="rId3"/>
+    <sheet name="documentation_reference" sheetId="7" r:id="rId4"/>
+    <sheet name="encounter" sheetId="1" r:id="rId5"/>
+    <sheet name="immunization" sheetId="10" r:id="rId6"/>
+    <sheet name="medication_statement" sheetId="5" r:id="rId7"/>
+    <sheet name="observation" sheetId="4" r:id="rId8"/>
+    <sheet name="organization" sheetId="9" r:id="rId9"/>
+    <sheet name="patient" sheetId="2" r:id="rId10"/>
+    <sheet name="practitioner" sheetId="8" r:id="rId11"/>
+    <sheet name="procedure" sheetId="6" r:id="rId12"/>
+    <sheet name="provenance" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="252">
   <si>
     <t xml:space="preserve"> Column        </t>
   </si>
@@ -658,9 +659,6 @@
     <t>Use to represent interactions between a patient and the healthcare system (outpatient, inpatient, etc.) in measure calculations.</t>
   </si>
   <si>
-    <t>condition</t>
-  </si>
-  <si>
     <t>Captures clinical diagnoses from FHIR Condition resources (e.g., SNOMED/ICD-10 codes).</t>
   </si>
   <si>
@@ -737,6 +735,75 @@
   </si>
   <si>
     <t>Use to attribute data to the correct institution, especially for multi-facility measure reporting.</t>
+  </si>
+  <si>
+    <t>condition_resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Description                                                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> claim_id        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> **Primary key**. FHIR `Claim.id`.                                                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Foreign key referencing `patient.patient_id`.                                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> status          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Claim status (`Claim.status`), e.g. active, cancelled, draft, entered-in-error.                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `Claim.type.coding[0].code` (e.g. institutional, professional).                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Display name for `Claim.type.coding[0].display`.                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sub_type_code   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Optional: `Claim.subType[0].coding[0].code`.                                                                </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sub_type_display</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Display for sub-type code.                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> use             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `Claim.use` (e.g. claim, preauthorization).                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TIMESTAMP    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> When the claim was created (`Claim.created`).                                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> total_value     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DECIMAL(10,2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total claim amount (`Claim.total.value`). Using a numeric/decimal field is often best for currency amounts. </t>
+  </si>
+  <si>
+    <t>claim</t>
+  </si>
+  <si>
+    <t>Stores claim details from FHIR Claim resources, including coverage and payment info. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Use to represent reimbursement requests or coverage claims. Can be used in measure calculations or for revenue cycle insights.</t>
   </si>
 </sst>
 </file>
@@ -803,8 +870,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B41DE9F6-D579-8944-80BC-1FB0CE9A511B}" name="Table1" displayName="Table1" ref="A1:C12" totalsRowShown="0">
-  <autoFilter ref="A1:C12" xr:uid="{B41DE9F6-D579-8944-80BC-1FB0CE9A511B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B41DE9F6-D579-8944-80BC-1FB0CE9A511B}" name="Table1" displayName="Table1" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13" xr:uid="{B41DE9F6-D579-8944-80BC-1FB0CE9A511B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
     <sortCondition ref="A1:A12"/>
   </sortState>
@@ -818,6 +885,18 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BFBB6F3C-F0BF-FF4B-8943-013DD3FB69AA}" name="Table9" displayName="Table9" ref="A1:C9" totalsRowShown="0">
+  <autoFilter ref="A1:C9" xr:uid="{BFBB6F3C-F0BF-FF4B-8943-013DD3FB69AA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8247F902-E0A3-904C-B137-0DC05B08B0ED}" name=" Column      "/>
+    <tableColumn id="2" xr3:uid="{3EA6D765-E85B-F34D-AA5B-F1CB86D48013}" name=" Type         "/>
+    <tableColumn id="3" xr3:uid="{A4EDC4B6-CDE7-C442-A4B5-A7F6BC55E8CB}" name=" Description                                                                 "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C0FAECB4-EF80-1C41-9409-878E9AA05020}" name="Table10" displayName="Table10" ref="A1:C10" totalsRowShown="0">
   <autoFilter ref="A1:C10" xr:uid="{C0FAECB4-EF80-1C41-9409-878E9AA05020}"/>
   <tableColumns count="3">
@@ -829,7 +908,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{46CFF17B-2BAD-B445-A4C2-629EEA0A23FC}" name="Table11" displayName="Table11" ref="A1:C8" totalsRowShown="0">
   <autoFilter ref="A1:C8" xr:uid="{46CFF17B-2BAD-B445-A4C2-629EEA0A23FC}"/>
   <tableColumns count="3">
@@ -841,7 +920,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{6EF48BCE-491E-0146-BC2B-6BE92E3C38FD}" name="Table12" displayName="Table12" ref="A1:C9" totalsRowShown="0">
   <autoFilter ref="A1:C9" xr:uid="{6EF48BCE-491E-0146-BC2B-6BE92E3C38FD}"/>
   <tableColumns count="3">
@@ -854,6 +933,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{C5170381-3B29-6747-B23F-CD946D6F1D13}" name="Table13" displayName="Table13" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11" xr:uid="{C5170381-3B29-6747-B23F-CD946D6F1D13}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F0046EDE-6B62-BC4A-9E42-640765BC80E2}" name=" Column          "/>
+    <tableColumn id="2" xr3:uid="{9BD0AD99-50BB-E948-8FA9-0150B4540755}" name=" Type         "/>
+    <tableColumn id="3" xr3:uid="{92BA7DE8-8DE5-EC41-AB2D-838D54454351}" name=" Description                                                                                                 "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{304EA665-2E12-4647-A6C3-EA4EBDAC6ECD}" name="Table2" displayName="Table2" ref="A1:C9" totalsRowShown="0">
   <autoFilter ref="A1:C9" xr:uid="{304EA665-2E12-4647-A6C3-EA4EBDAC6ECD}"/>
   <tableColumns count="3">
@@ -865,7 +956,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6E3E59E5-3B84-E644-A828-9F574DB049AB}" name="Table3" displayName="Table3" ref="A1:C11" totalsRowShown="0">
   <autoFilter ref="A1:C11" xr:uid="{6E3E59E5-3B84-E644-A828-9F574DB049AB}"/>
   <tableColumns count="3">
@@ -877,7 +968,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0C82846C-F5DF-E84B-800F-67822C85A102}" name="Table4" displayName="Table4" ref="A1:C7" totalsRowShown="0">
   <autoFilter ref="A1:C7" xr:uid="{0C82846C-F5DF-E84B-800F-67822C85A102}"/>
   <tableColumns count="3">
@@ -889,7 +980,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C381BDC8-851C-4544-A92E-1C4502582A6E}" name="Table5" displayName="Table5" ref="A1:C10" totalsRowShown="0">
   <autoFilter ref="A1:C10" xr:uid="{C381BDC8-851C-4544-A92E-1C4502582A6E}"/>
   <tableColumns count="3">
@@ -901,7 +992,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EC726791-35F0-7945-8475-78D227DF1F19}" name="Table6" displayName="Table6" ref="A1:C9" totalsRowShown="0">
   <autoFilter ref="A1:C9" xr:uid="{EC726791-35F0-7945-8475-78D227DF1F19}"/>
   <tableColumns count="3">
@@ -913,7 +1004,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D7D0BA23-D339-9C40-BF69-12D65F74647E}" name="Table7" displayName="Table7" ref="A1:C10" totalsRowShown="0">
   <autoFilter ref="A1:C10" xr:uid="{D7D0BA23-D339-9C40-BF69-12D65F74647E}"/>
   <tableColumns count="3">
@@ -925,25 +1016,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C50F4A7-A424-464D-AAA7-82FA1E0DF1A3}" name="Table8" displayName="Table8" ref="A1:C8" totalsRowShown="0">
   <autoFilter ref="A1:C8" xr:uid="{5C50F4A7-A424-464D-AAA7-82FA1E0DF1A3}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8132AAD2-7FED-1145-A853-5EB374DBDB80}" name=" Column           "/>
     <tableColumn id="2" xr3:uid="{0072E864-0F62-A24E-9712-777694EC5A77}" name=" Type         "/>
     <tableColumn id="3" xr3:uid="{92A321FA-671E-934F-89DC-6D133289BC49}" name=" Description                                                                    "/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BFBB6F3C-F0BF-FF4B-8943-013DD3FB69AA}" name="Table9" displayName="Table9" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9" xr:uid="{BFBB6F3C-F0BF-FF4B-8943-013DD3FB69AA}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8247F902-E0A3-904C-B137-0DC05B08B0ED}" name=" Column      "/>
-    <tableColumn id="2" xr3:uid="{3EA6D765-E85B-F34D-AA5B-F1CB86D48013}" name=" Type         "/>
-    <tableColumn id="3" xr3:uid="{A4EDC4B6-CDE7-C442-A4B5-A7F6BC55E8CB}" name=" Description                                                                 "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1266,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24989AB3-C241-3B4C-B9CC-AE55414D9C9E}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1292,24 +1371,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" t="s">
         <v>203</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>204</v>
-      </c>
-      <c r="C2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" t="s">
         <v>215</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>216</v>
-      </c>
-      <c r="C3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,46 +1404,46 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" t="s">
         <v>221</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>222</v>
-      </c>
-      <c r="C5" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B6" t="s">
         <v>209</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>210</v>
-      </c>
-      <c r="C6" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" t="s">
         <v>206</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>207</v>
-      </c>
-      <c r="C7" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" t="s">
         <v>227</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>228</v>
-      </c>
-      <c r="C8" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1380,35 +1459,46 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" t="s">
         <v>224</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>225</v>
-      </c>
-      <c r="C10" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" t="s">
         <v>212</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>213</v>
-      </c>
-      <c r="C11" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" t="s">
         <v>218</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>219</v>
       </c>
-      <c r="C12" t="s">
-        <v>220</v>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -1424,7 +1514,131 @@
     <hyperlink ref="A10" location="practitioner!A1" display="practitioner" xr:uid="{3366B8DD-C6BF-7443-9486-293E2C4C2DAD}"/>
     <hyperlink ref="A11" location="procedure!A1" display="procedure" xr:uid="{27DFF5EE-914A-C949-883D-25E30404EC02}"/>
     <hyperlink ref="A12" location="provenance!A1" display="provenance" xr:uid="{3B3B4E88-C4B4-3B47-8D55-6E8F813AFDCC}"/>
+    <hyperlink ref="A13" location="claim!A1" display="claim" xr:uid="{E1C6EA58-06FB-8B40-B4D7-AB85645B6C0A}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED5E86A-994C-2B46-A705-C1B7BA10D697}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1432,7 +1646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A2A75C-D5B6-3D4E-A5C0-F059837FED53}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -1565,7 +1779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F7B6D48-00E2-A545-8A9E-FB38463F2399}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1676,7 +1890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7994913-2C7E-F641-BE0F-DE6C072C6494}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1799,6 +2013,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E741891B-AD06-DC43-B7EF-07E47568D12C}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>244</v>
+      </c>
+      <c r="C10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EEBB009-3E72-3B43-8091-7DCDD17DE4EA}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1920,12 +2278,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FF0737-1FBE-3146-BEED-76A41B290D46}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScale="174" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2064,7 +2422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5908863-A096-3648-BDDF-A2531564C03E}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2164,7 +2522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{281461CC-6740-4D43-B01A-1A9CC883F51C}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -2297,7 +2655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E43A89-ABCA-674E-8A48-328BA4F5F3AF}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2419,7 +2777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE28832-A11F-324A-AF0A-31612357C0CE}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -2552,7 +2910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B42F7E9-F312-EE40-8E99-9C2FFC7DC5B9}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2661,126 +3019,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED5E86A-994C-2B46-A705-C1B7BA10D697}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>